<commit_message>
fpspreadsheet: Fix format in predefined test files (test*_1899*.* and test*_1904*.*); fix biff8 ignoring cell format in shared formula range.
git-svn-id: http://svn.code.sf.net/p/lazarus-ccr/svn@4108 8e941d3f-bd1b-0410-a28a-d453659cc2b4
</commit_message>
<xml_diff>
--- a/components/fpspreadsheet/tests/testooxml_1899.xlsx
+++ b/components/fpspreadsheet/tests/testooxml_1899.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Numbers" sheetId="1" r:id="rId1"/>
@@ -126,12 +126,6 @@
     <t>formatted as nfLongTimeAM</t>
   </si>
   <si>
-    <t>formatted as nfFmtDateTime, dm</t>
-  </si>
-  <si>
-    <t>formatted as nfFmtDateTime, my</t>
-  </si>
-  <si>
     <t>formatted as nfFmtDateTime, ms</t>
   </si>
   <si>
@@ -169,21 +163,28 @@
   </si>
   <si>
     <t>minus 59 million + 0.1234, formatted as "currencyRed" with 2 decimals, brackets and EUR</t>
+  </si>
+  <si>
+    <t>formatted as nfDayMonth</t>
+  </si>
+  <si>
+    <t>formatted as nfMonthYear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="173" formatCode="h:mm;@"/>
-    <numFmt numFmtId="174" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="175" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="176" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="178" formatCode="#,##0.00\ [$$-409]"/>
-    <numFmt numFmtId="179" formatCode="[$$-409]#,##0.00;[Red]\-#,###.00\ [$$-409]"/>
-    <numFmt numFmtId="181" formatCode="#,##0.00\ [$EUR];[Red]\(#,##0.00\ [$EUR]\)"/>
+  <numFmts count="9">
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="167" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00\ [$$-409]"/>
+    <numFmt numFmtId="170" formatCode="[$$-409]#,##0.00;[Red]\-#,###.00\ [$$-409]"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00\ [$EUR];[Red]\(#,##0.00\ [$EUR]\)"/>
+    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd\Thh:mm:ss"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -223,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -233,10 +234,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -244,13 +245,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -258,9 +260,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,7 +300,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -368,7 +370,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -544,11 +546,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -657,7 +659,7 @@
         <v>0.35360000000000003</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -665,7 +667,7 @@
         <v>0.35360000000000003</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -697,7 +699,7 @@
         <v>59000000.123400003</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -705,7 +707,7 @@
         <v>59000000.123400003</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -713,7 +715,7 @@
         <v>-59000000.123400003</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -721,7 +723,7 @@
         <v>-59000000.123400003</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -729,7 +731,7 @@
         <v>-59000000.123400003</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -749,9 +751,9 @@
       <selection activeCell="A12" sqref="A12:IV12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="1" max="1" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -815,7 +817,7 @@
         <v>0.35360000000000003</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -823,7 +825,7 @@
         <v>0.35360000000000003</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -855,7 +857,7 @@
         <v>59000000.123400003</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -863,7 +865,7 @@
         <v>-59000000.123400003</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -879,16 +881,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="18.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+    <col min="1" max="1" width="18.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -896,9 +898,9 @@
         <v>2082</v>
       </c>
       <c r="B1" s="17"/>
-      <c r="C1" t="str">
-        <f>TEXT(A1,"yyyy\-mm\-ddThh\:mm\:ss")</f>
-        <v>yyyy-00-dd1200:00:00</v>
+      <c r="C1" s="24">
+        <f t="shared" ref="C1:C35" si="0">A1</f>
+        <v>2082</v>
       </c>
       <c r="D1" t="s">
         <v>23</v>
@@ -912,9 +914,9 @@
         <v>3178.5</v>
       </c>
       <c r="B2" s="17"/>
-      <c r="C2" t="str">
-        <f t="shared" ref="C2:C36" si="0">TEXT(A2,"yyyy\-mm\-ddThh\:mm\:ss")</f>
-        <v>yyyy-00-dd1212:00:00</v>
+      <c r="C2" s="24">
+        <f t="shared" si="0"/>
+        <v>3178.5</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -928,9 +930,9 @@
         <v>41602</v>
       </c>
       <c r="B3" s="17"/>
-      <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd2400:00:00</v>
+      <c r="C3" s="24">
+        <f t="shared" si="0"/>
+        <v>41602</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
@@ -941,9 +943,9 @@
         <v>47848</v>
       </c>
       <c r="B4" s="17"/>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd3100:00:00</v>
+      <c r="C4" s="24">
+        <f t="shared" si="0"/>
+        <v>47848</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -951,9 +953,9 @@
         <v>0</v>
       </c>
       <c r="B5" s="17"/>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:00</v>
+      <c r="C5" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -964,9 +966,9 @@
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="B6" s="17"/>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:01</v>
+      <c r="C6" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -977,9 +979,9 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="B7" s="17"/>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd001:00:00</v>
+      <c r="C7" s="24">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -987,9 +989,9 @@
         <v>0.125</v>
       </c>
       <c r="B8" s="17"/>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd003:00:00</v>
+      <c r="C8" s="24">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -997,9 +999,9 @@
         <v>0.5</v>
       </c>
       <c r="B9" s="17"/>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd012:00:00</v>
+      <c r="C9" s="24">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -1010,9 +1012,9 @@
         <v>0.75</v>
       </c>
       <c r="B10" s="17"/>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd018:00:00</v>
+      <c r="C10" s="24">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1020,9 +1022,9 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="B11" s="17"/>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:00</v>
+      <c r="C11" s="24">
+        <f t="shared" si="0"/>
+        <v>0.99930555555555556</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1030,9 +1032,9 @@
         <v>0.99998842592592585</v>
       </c>
       <c r="B12" s="17"/>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:59</v>
+      <c r="C12" s="24">
+        <f t="shared" si="0"/>
+        <v>0.99998842592592585</v>
       </c>
       <c r="D12" t="s">
         <v>27</v>
@@ -1043,9 +1045,9 @@
         <v>3178.5</v>
       </c>
       <c r="B13" s="17"/>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd1212:00:00</v>
+      <c r="C13" s="24">
+        <f t="shared" si="0"/>
+        <v>3178.5</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
@@ -1059,9 +1061,9 @@
         <v>3178.5</v>
       </c>
       <c r="B14" s="17"/>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd1212:00:00</v>
+      <c r="C14" s="24">
+        <f t="shared" si="0"/>
+        <v>3178.5</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
@@ -1075,9 +1077,9 @@
         <v>3178.5</v>
       </c>
       <c r="B15" s="17"/>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd1212:00:00</v>
+      <c r="C15" s="24">
+        <f t="shared" si="0"/>
+        <v>3178.5</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
@@ -1091,9 +1093,9 @@
         <v>3178.5</v>
       </c>
       <c r="B16" s="17"/>
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd1212:00:00</v>
+      <c r="C16" s="24">
+        <f t="shared" si="0"/>
+        <v>3178.5</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
@@ -1107,9 +1109,9 @@
         <v>3178.5</v>
       </c>
       <c r="B17" s="17"/>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd1212:00:00</v>
+      <c r="C17" s="24">
+        <f t="shared" si="0"/>
+        <v>3178.5</v>
       </c>
       <c r="D17" t="s">
         <v>24</v>
@@ -1123,15 +1125,15 @@
         <v>3178.5</v>
       </c>
       <c r="B18" s="17"/>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd1212:00:00</v>
+      <c r="C18" s="24">
+        <f t="shared" si="0"/>
+        <v>3178.5</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1139,15 +1141,15 @@
         <v>3178.5</v>
       </c>
       <c r="B19" s="17"/>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd1212:00:00</v>
+      <c r="C19" s="24">
+        <f t="shared" si="0"/>
+        <v>3178.5</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1155,15 +1157,15 @@
         <v>3178.5</v>
       </c>
       <c r="B20" s="17"/>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd1212:00:00</v>
+      <c r="C20" s="24">
+        <f t="shared" si="0"/>
+        <v>3178.5</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1171,9 +1173,9 @@
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="B21" s="17"/>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:01</v>
+      <c r="C21" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D21" t="s">
         <v>26</v>
@@ -1187,9 +1189,9 @@
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="B22" s="17"/>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:01</v>
+      <c r="C22" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
@@ -1203,9 +1205,9 @@
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="B23" s="17"/>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:01</v>
+      <c r="C23" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D23" t="s">
         <v>26</v>
@@ -1219,9 +1221,9 @@
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="B24" s="17"/>
-      <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:01</v>
+      <c r="C24" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1235,9 +1237,9 @@
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="B25" s="17"/>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:01</v>
+      <c r="C25" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
@@ -1251,15 +1253,15 @@
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="B26" s="17"/>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:01</v>
+      <c r="C26" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1267,15 +1269,15 @@
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="B27" s="17"/>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:01</v>
+      <c r="C27" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D27" t="s">
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1283,15 +1285,15 @@
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="B28" s="17"/>
-      <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-00-dd000:00:01</v>
+      <c r="C28" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D28" t="s">
         <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1299,9 +1301,9 @@
         <v>0.99998842592592585</v>
       </c>
       <c r="B29" s="17"/>
-      <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:59</v>
+      <c r="C29" s="24">
+        <f t="shared" si="0"/>
+        <v>0.99998842592592585</v>
       </c>
       <c r="D29" t="s">
         <v>27</v>
@@ -1315,9 +1317,9 @@
         <v>0.99998842592592585</v>
       </c>
       <c r="B30" s="17"/>
-      <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:59</v>
+      <c r="C30" s="24">
+        <f t="shared" si="0"/>
+        <v>0.99998842592592585</v>
       </c>
       <c r="D30" t="s">
         <v>27</v>
@@ -1331,9 +1333,9 @@
         <v>0.99998842592592585</v>
       </c>
       <c r="B31" s="17"/>
-      <c r="C31" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:59</v>
+      <c r="C31" s="24">
+        <f t="shared" si="0"/>
+        <v>0.99998842592592585</v>
       </c>
       <c r="D31" t="s">
         <v>27</v>
@@ -1347,9 +1349,9 @@
         <v>0.99998842592592585</v>
       </c>
       <c r="B32" s="17"/>
-      <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:59</v>
+      <c r="C32" s="24">
+        <f t="shared" si="0"/>
+        <v>0.99998842592592585</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -1363,9 +1365,9 @@
         <v>0.99998842592592585</v>
       </c>
       <c r="B33" s="17"/>
-      <c r="C33" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:59</v>
+      <c r="C33" s="24">
+        <f t="shared" si="0"/>
+        <v>0.99998842592592585</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
@@ -1379,15 +1381,15 @@
         <v>0.99998842592592585</v>
       </c>
       <c r="B34" s="17"/>
-      <c r="C34" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:59</v>
+      <c r="C34" s="24">
+        <f t="shared" si="0"/>
+        <v>0.99998842592592585</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1395,15 +1397,15 @@
         <v>0.99998842592592585</v>
       </c>
       <c r="B35" s="17"/>
-      <c r="C35" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:59</v>
+      <c r="C35" s="24">
+        <f t="shared" si="0"/>
+        <v>0.99998842592592585</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1411,15 +1413,15 @@
         <v>0.99998842592592585</v>
       </c>
       <c r="B36" s="17"/>
-      <c r="C36" t="str">
-        <f t="shared" si="0"/>
-        <v>yyyy-59-dd023:59:59</v>
+      <c r="C36" s="24">
+        <f>A36</f>
+        <v>0.99998842592592585</v>
       </c>
       <c r="D36" t="s">
         <v>27</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1428,10 +1430,10 @@
       </c>
       <c r="B37" s="17"/>
       <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
         <v>39</v>
-      </c>
-      <c r="E37" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1440,10 +1442,10 @@
       </c>
       <c r="B38" s="17"/>
       <c r="C38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>